<commit_message>
add insert file funcion and clean code
</commit_message>
<xml_diff>
--- a/public/files/resume_insert_template.xlsx
+++ b/public/files/resume_insert_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SINAU\designyeuh-web\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513B2B5C-FB16-4F0B-9FC5-57B3E7E48533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52C56C0-D197-4F98-9E00-E51C4D00720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{25E1AAA0-BA6B-40EB-BEE7-24E92C59A128}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,7 +463,7 @@
     <col min="3" max="3" width="31.26953125" style="7" customWidth="1"/>
     <col min="4" max="4" width="18.6328125" style="7" customWidth="1"/>
     <col min="5" max="5" width="20.54296875" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="1" hidden="1"/>
+    <col min="6" max="6" width="20.54296875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" style="1" hidden="1"/>
   </cols>
   <sheetData>

</xml_diff>